<commit_message>
Added notebook for fetching synonyms
</commit_message>
<xml_diff>
--- a/benchmarks/Benchmark.xlsx
+++ b/benchmarks/Benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F423AB66-4203-4BF1-88E9-A209D843D831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB5982E-6398-41C2-9DAB-FCF82C370FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1908,10 +1908,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4578,11 +4578,6 @@
       <c r="G92" s="12"/>
       <c r="J92" s="12" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A93" s="12">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>